<commit_message>
Fixed FMBN 5.1.2 (early release)
Fixed a few problems with edges and added two studies on olives
</commit_message>
<xml_diff>
--- a/the_real_thing/FMBN_5/Excel_text_files_v5/Abstracts.xlsx
+++ b/the_real_thing/FMBN_5/Excel_text_files_v5/Abstracts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenioparente/Library/CloudStorage/GoogleDrive-eugenio.parente@unibas.it/My Drive/FMBN/FMBNv5/FMBN_5_1/FMBN5_1_1_060525/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenioparente/Library/CloudStorage/GoogleDrive-eugenio.parente@unibas.it/My Drive/FMBN/FMBNv5/FMBN_5_1_2/FMBN_5_1_2_100925/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F057AC3-9ECA-4547-ABE1-42FD0C3B75A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C017EEE6-9D5B-EA45-908E-E9493DD341DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="500" windowWidth="31940" windowHeight="17560" xr2:uid="{EC83DC76-DA63-8B42-8906-4BAF203BC638}"/>
+    <workbookView xWindow="4780" yWindow="500" windowWidth="34080" windowHeight="19200" xr2:uid="{EC83DC76-DA63-8B42-8906-4BAF203BC638}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="582">
   <si>
     <t>study</t>
   </si>
@@ -1777,6 +1777,15 @@
   </si>
   <si>
     <t>Agiorgitiko is a major Greek red winegrape variety of high economic importance cultivated almost exclusively in the Nemea PDO zone in Peloponnese, Greece. Here, we describe the microbiota and mycobiota of grape and soil samples collected over three consecutive harvest periods (September 2019, 2020 and 2021). The results revealed a common microbiome composition across the Nemea PDO zone vineyards, despite significant variations in the community structure regarding dominant bacterial and fungal taxa per sampling year, which were associated with weather factors. Grape samples of 2019 were enriched in several plant growth promoting bacteria, including Bradyrhizobium, Streptomyces, Massilia and Sphingomonas, selected by the particular weather conditions. On the other hand, the predominance of Botrytis in the same samples was observed, indicating again the impact of weather conditions on the microbial structure. Understanding these dynamics could improve management practices aimed at vine cultivation and wine quality.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ijfoodmicro.2025.111332</t>
+  </si>
+  <si>
+    <t>The microbial terroir of Greek olive varieties remains underexplored. In this study, 62 samples of olive fruits, collected across the harvest period 2019–2020, were analyzed by high-throughput sequencing. The samples represented 38 olive varieties collected from geographically well distributed regions of Greece. Analysis of the bacterial composition revealed that the geographical area was a significant factor in discriminating samples. The core microbiota included Erwinia, Pseudomonas, and members of the Enterobacteriaceae family. Furthermore, a notable variation in bacterial taxa abundances associated with the geographic location was observed. The sampling area was a key discriminant factor for the mycobiota, and the core mycobiota comprised Alternaria, Taphrina, Candida, Wickerhamomyces anomalus and Penicillium. Finally, Redundancy Analysis (RDA) revealed a notable association between environmental characteristics and microbial composition. Specifically, tree age was associated with certain bacterial and fungal taxa (Pearson's correlation p-value adj.[FDR] &lt; 0.05).</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -2168,13 +2177,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0F821E-4D0E-9C48-880F-AED2209EDDE4}">
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C303"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D301" sqref="D301"/>
+      <selection pane="bottomRight" activeCell="C303" sqref="A1:C303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5491,6 +5500,28 @@
         <v>578</v>
       </c>
     </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>301</v>
+      </c>
+      <c r="B302" t="s">
+        <v>579</v>
+      </c>
+      <c r="C302" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>302</v>
+      </c>
+      <c r="B303" t="s">
+        <v>581</v>
+      </c>
+      <c r="C303" t="s">
+        <v>581</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C234" xr:uid="{0F0F821E-4D0E-9C48-880F-AED2209EDDE4}"/>
   <hyperlinks>

</xml_diff>